<commit_message>
add excelutilities under code changes
</commit_message>
<xml_diff>
--- a/Test_data/login_test_data.xlsx
+++ b/Test_data/login_test_data.xlsx
@@ -7,17 +7,29 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
   <si>
     <t>admin@yourstore.com</t>
   </si>
@@ -25,25 +37,16 @@
     <t>admin</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>admistore.com</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>adm</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>exp</t>
-  </si>
-  <si>
-    <t>user</t>
   </si>
   <si>
     <t>admin@yourst.com</t>
@@ -56,7 +59,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +79,13 @@
       <color rgb="FF067D17"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -118,17 +128,19 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,60 +449,67 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3" s="6"/>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -498,7 +517,7 @@
     <hyperlink ref="A5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 

</xml_diff>